<commit_message>
UPDATE CLIENT MONSTER & PLAYER STATUS
</commit_message>
<xml_diff>
--- a/2차 설계서/레벨 디자인 문서.xlsx
+++ b/2차 설계서/레벨 디자인 문서.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\FairyTaleVirus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\FairyTaleVirus\FairyTaleVirus\2차 설계서\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C8D04F-ABFA-4D44-995E-B49511709630}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{C8E4037B-B5A9-45C2-9088-3C8AB462B2E7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="1" xr2:uid="{C8E4037B-B5A9-45C2-9088-3C8AB462B2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
     <sheet name="character" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>오염도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,6 +213,110 @@
   </si>
   <si>
     <t>난이도보정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 기본 스탯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가중치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앨리스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간망토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격속도 = 몬스터 생성속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5대로 계산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1인기준 사서의 물리대미지 기준 2방</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력 = 본인, 정신 = 버프 효과 ^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7스테이지 기준</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp = 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>((x-1)2 / 5 + 1)*40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 1.5, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20, 15, 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -688,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF3E8D6-B221-4C58-8F9A-BF823B1B0E9B}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1873,17 +1978,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2111EC-E7F6-490B-9D83-A3B7AA7DCCEC}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.75" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
+    <col min="8" max="8" width="6.25" customWidth="1"/>
     <col min="10" max="10" width="14.25" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="17.875" customWidth="1"/>
@@ -2039,7 +2146,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">90*C3*B3</f>
+        <f t="shared" ref="D3:D5" si="0">90*C3*B3</f>
         <v>3420</v>
       </c>
       <c r="E3">
@@ -3118,6 +3225,431 @@
       <c r="O20">
         <f t="shared" si="36"/>
         <v>2707.7142857142858</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>46</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>80</v>
+      </c>
+      <c r="H32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>40</v>
+      </c>
+      <c r="D33">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>40</v>
+      </c>
+      <c r="G33">
+        <v>60</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <f>1+B36/10</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D36">
+        <f>1 + ((B36-1)*(B36-1)/4 + 1)/10</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E36">
+        <f>40*C36</f>
+        <v>44</v>
+      </c>
+      <c r="F36">
+        <f>40*D36</f>
+        <v>44</v>
+      </c>
+      <c r="G36">
+        <v>80</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:C43" si="37">1+B37/10</f>
+        <v>1.2</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:D43" si="38">1 + ((B37-1)*(B37-1)/4 + 1)/10</f>
+        <v>1.125</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ref="E37:F43" si="39">40*C37</f>
+        <v>48</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="39"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="37"/>
+        <v>1.3</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="38"/>
+        <v>1.2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="39"/>
+        <v>52</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="39"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="37"/>
+        <v>1.4</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="38"/>
+        <v>1.325</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="39"/>
+        <v>56</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="39"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="37"/>
+        <v>1.5</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="38"/>
+        <v>1.5</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="39"/>
+        <v>60</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="39"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="37"/>
+        <v>1.6</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="38"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="39"/>
+        <v>64</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="39"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="37"/>
+        <v>1.7</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="39"/>
+        <v>68</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="39"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="37"/>
+        <v>1.8</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="38"/>
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="39"/>
+        <v>72</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="39"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E47">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>3.6</v>
+      </c>
+      <c r="E48">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>5.2</v>
+      </c>
+      <c r="E49">
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>